<commit_message>
utilisation du decorator et des style tailwindcss dans application.tailwind.css
</commit_message>
<xml_diff>
--- a/public/agents.xlsx
+++ b/public/agents.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,6 +558,36 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>moctar</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>moctar@exemple.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>B19</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Vice-Président</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>